<commit_message>
fix template: show all pembayaran history
</commit_message>
<xml_diff>
--- a/writable/templates/template_cetak_pembayaran_by_mhs.xlsx
+++ b/writable/templates/template_cetak_pembayaran_by_mhs.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>DETAIL PEMBAYARAN MAHASISWA</t>
   </si>
@@ -32,6 +33,12 @@
   </si>
   <si>
     <t>SISA TAGIHAN ITEM</t>
+  </si>
+  <si>
+    <t>NOMINAL PEMBAYARAN</t>
+  </si>
+  <si>
+    <t>TANGGAL PEMBAYARAN</t>
   </si>
 </sst>
 </file>
@@ -67,7 +74,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -81,6 +88,9 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -90,6 +100,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -28320,4 +28334,75 @@
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="39.71"/>
+    <col customWidth="1" min="2" max="2" width="22.71"/>
+    <col customWidth="1" min="3" max="3" width="27.71"/>
+    <col customWidth="1" min="4" max="4" width="28.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>